<commit_message>
Added emails to excel
</commit_message>
<xml_diff>
--- a/emails_validatedd.xlsx
+++ b/emails_validatedd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinthalwarsaideekshith/Desktop/Auto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317FD54C-E394-0D47-8B6A-39BA0CDB725F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C74EE53-F4A7-1741-9CF5-E799A2673546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="272">
   <si>
     <t>Company</t>
   </si>
@@ -834,6 +834,9 @@
   </si>
   <si>
     <t>saidekshith1200@gmail.com</t>
+  </si>
+  <si>
+    <t>saideekshith1200@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1213,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1228,12 +1231,12 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{6811B8CE-D01B-2846-B7A5-214564026849}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{CB79CB42-2746-5440-916A-907773D31BDC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1241,7 +1244,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2358,6 +2361,11 @@
         <v>269</v>
       </c>
     </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>